<commit_message>
Revised lecture notes and lab assignment
</commit_message>
<xml_diff>
--- a/Labs/Lab01/CS133JS_Lab01_Rubrics.xlsx
+++ b/Labs/Lab01/CS133JS_Lab01_Rubrics.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/DataCard/Repos/CS133JS-CourseMaterials/Labs/Lab01/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/birdb/Projects/CS133JS-CourseMaterials/Labs/Lab01/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{292B7E0A-C394-4240-8FC5-DDAD0D47954D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEF6249A-D3E9-D543-A50C-F482CA0D5295}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="320" yWindow="1400" windowWidth="12600" windowHeight="14520" activeTab="2" xr2:uid="{9702CE45-50CE-F14F-802C-E5FE921247A2}"/>
+    <workbookView xWindow="-13500" yWindow="3540" windowWidth="13500" windowHeight="14520" activeTab="1" xr2:uid="{9702CE45-50CE-F14F-802C-E5FE921247A2}"/>
   </bookViews>
   <sheets>
     <sheet name="Group A" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="34">
   <si>
     <t>Criteria</t>
   </si>
@@ -123,6 +123,12 @@
   </si>
   <si>
     <t>Part A: Exercise</t>
+  </si>
+  <si>
+    <t>Part 1: Exercise</t>
+  </si>
+  <si>
+    <t>Part 2</t>
   </si>
 </sst>
 </file>
@@ -496,12 +502,14 @@
   <dimension ref="A1:E18"/>
   <sheetViews>
     <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="3" max="3" width="17.6640625" customWidth="1"/>
+    <col min="3" max="3" width="22.33203125" customWidth="1"/>
+    <col min="4" max="4" width="8.1640625" customWidth="1"/>
+    <col min="5" max="5" width="6.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
@@ -525,14 +533,14 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
-      <c r="D4" s="3">
+      <c r="D4">
         <v>10</v>
       </c>
-      <c r="E4" s="3">
+      <c r="E4">
         <v>10</v>
       </c>
     </row>
@@ -540,25 +548,21 @@
       <c r="A5" s="3"/>
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
+        <v>33</v>
+      </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>26</v>
       </c>
       <c r="D7">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E7">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
@@ -566,10 +570,10 @@
         <v>9</v>
       </c>
       <c r="D8">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E8">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
@@ -577,10 +581,10 @@
         <v>2</v>
       </c>
       <c r="D9">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E9">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
@@ -588,10 +592,10 @@
         <v>3</v>
       </c>
       <c r="D10">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E10">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
@@ -599,10 +603,10 @@
         <v>21</v>
       </c>
       <c r="D11">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="E11">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
@@ -610,10 +614,10 @@
         <v>4</v>
       </c>
       <c r="D12">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E12">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
@@ -621,10 +625,10 @@
         <v>10</v>
       </c>
       <c r="D13">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E13">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
@@ -643,10 +647,10 @@
         <v>5</v>
       </c>
       <c r="D15">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E15">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
@@ -654,10 +658,10 @@
         <v>29</v>
       </c>
       <c r="D16">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E16">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
@@ -666,11 +670,11 @@
       </c>
       <c r="D18">
         <f>SUM(D3:D16)</f>
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="E18">
         <f>SUM(E3:E16)</f>
-        <v>50</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>
@@ -682,8 +686,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D6A7069-CD8C-C44F-B7C6-148A7A61DB13}">
   <dimension ref="A1:E18"/>
   <sheetViews>
-    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -716,10 +720,10 @@
       </c>
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
-      <c r="D4" s="3">
+      <c r="D4">
         <v>10</v>
       </c>
-      <c r="E4" s="3">
+      <c r="E4">
         <v>10</v>
       </c>
     </row>
@@ -727,25 +731,21 @@
       <c r="A5" s="3"/>
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>26</v>
       </c>
       <c r="D7">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E7">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
@@ -753,10 +753,10 @@
         <v>9</v>
       </c>
       <c r="D8">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E8">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
@@ -764,10 +764,10 @@
         <v>13</v>
       </c>
       <c r="D9">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E9">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
@@ -775,10 +775,10 @@
         <v>14</v>
       </c>
       <c r="D10">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E10">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
@@ -786,10 +786,10 @@
         <v>20</v>
       </c>
       <c r="D11">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="E11">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
@@ -797,10 +797,10 @@
         <v>19</v>
       </c>
       <c r="D12">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E12">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
@@ -808,10 +808,10 @@
         <v>28</v>
       </c>
       <c r="D13">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E13">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
@@ -830,10 +830,10 @@
         <v>5</v>
       </c>
       <c r="D15">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E15">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
@@ -841,10 +841,10 @@
         <v>29</v>
       </c>
       <c r="D16">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E16">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
@@ -853,11 +853,11 @@
       </c>
       <c r="D18">
         <f>SUM(D3:D16)</f>
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="E18">
         <f>SUM(E3:E16)</f>
-        <v>50</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>
@@ -869,13 +869,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A23F5BD0-DC32-2447-A1C1-D2E07E467E1B}">
   <dimension ref="A1:E18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4:E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="3" max="3" width="21.6640625" customWidth="1"/>
+    <col min="3" max="3" width="22.5" customWidth="1"/>
+    <col min="4" max="4" width="8" customWidth="1"/>
+    <col min="5" max="5" width="6.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
@@ -899,14 +901,14 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
-      <c r="D4" s="3">
+      <c r="D4">
         <v>10</v>
       </c>
-      <c r="E4" s="3">
+      <c r="E4">
         <v>10</v>
       </c>
     </row>
@@ -914,25 +916,21 @@
       <c r="A5" s="3"/>
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
+        <v>33</v>
+      </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>26</v>
       </c>
       <c r="D7">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E7">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
@@ -940,10 +938,10 @@
         <v>9</v>
       </c>
       <c r="D8">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E8">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
@@ -951,10 +949,10 @@
         <v>17</v>
       </c>
       <c r="D9">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E9">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
@@ -962,10 +960,10 @@
         <v>18</v>
       </c>
       <c r="D10">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E10">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
@@ -973,10 +971,10 @@
         <v>25</v>
       </c>
       <c r="D11">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="E11">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
@@ -984,10 +982,10 @@
         <v>22</v>
       </c>
       <c r="D12">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E12">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
@@ -995,10 +993,10 @@
         <v>23</v>
       </c>
       <c r="D13">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E13">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
@@ -1017,10 +1015,10 @@
         <v>27</v>
       </c>
       <c r="D15">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E15">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
@@ -1028,10 +1026,10 @@
         <v>29</v>
       </c>
       <c r="D16">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E16">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
@@ -1040,11 +1038,11 @@
       </c>
       <c r="D18">
         <f>SUM(D3:D16)</f>
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="E18">
         <f>SUM(E3:E16)</f>
-        <v>50</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated lab 1 rubric formatting
</commit_message>
<xml_diff>
--- a/Labs/Lab01/CS133JS_Lab01_Rubrics.xlsx
+++ b/Labs/Lab01/CS133JS_Lab01_Rubrics.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11008"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/birdb/Projects/CS133JS-CourseMaterials/Labs/Lab01/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/brian/Repos/CS133JS-CourseMaterials/Labs/Lab01/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9833D7FE-4B10-6F40-9884-0B9803CCDB39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{608BF223-3486-724D-AC91-A40DAA5252E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-25220" yWindow="2420" windowWidth="24580" windowHeight="15400" xr2:uid="{9702CE45-50CE-F14F-802C-E5FE921247A2}"/>
+    <workbookView xWindow="13500" yWindow="980" windowWidth="12740" windowHeight="15040" xr2:uid="{9702CE45-50CE-F14F-802C-E5FE921247A2}"/>
   </bookViews>
   <sheets>
     <sheet name="Group A" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="39">
   <si>
     <t>Criteria</t>
   </si>
@@ -149,6 +149,12 @@
   </si>
   <si>
     <t>Here's the grading breakdown:</t>
+  </si>
+  <si>
+    <t>Excellent work!</t>
+  </si>
+  <si>
+    <t>Comments</t>
   </si>
 </sst>
 </file>
@@ -200,11 +206,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -223,9 +235,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -263,7 +275,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -369,7 +381,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -511,7 +523,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -519,10 +531,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3216228F-B421-8943-9C69-C9FAC1E7C520}">
-  <dimension ref="A1:E19"/>
+  <dimension ref="A1:G19"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -530,30 +542,33 @@
     <col min="3" max="3" width="22.33203125" customWidth="1"/>
     <col min="4" max="4" width="8.1640625" customWidth="1"/>
     <col min="5" max="5" width="6.1640625" customWidth="1"/>
+    <col min="6" max="6" width="1.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" s="3" t="s">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="B2" s="5"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" s="3"/>
-      <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B3" s="5"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="5"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>0</v>
       </c>
@@ -563,8 +578,11 @@
       <c r="E4" s="2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G4" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>32</v>
       </c>
@@ -576,17 +594,23 @@
       <c r="E5">
         <v>10</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F5" s="4"/>
+      <c r="G5" s="4"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F6" s="4"/>
+      <c r="G6" s="4"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F7" s="4"/>
+      <c r="G7" s="4"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>26</v>
       </c>
@@ -596,8 +620,10 @@
       <c r="E8">
         <v>2</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F8" s="4"/>
+      <c r="G8" s="4"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -607,8 +633,10 @@
       <c r="E9">
         <v>3</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F9" s="4"/>
+      <c r="G9" s="4"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>2</v>
       </c>
@@ -618,8 +646,10 @@
       <c r="E10">
         <v>4</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F10" s="4"/>
+      <c r="G10" s="4"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>3</v>
       </c>
@@ -629,8 +659,10 @@
       <c r="E11">
         <v>4</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F11" s="4"/>
+      <c r="G11" s="4"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>21</v>
       </c>
@@ -640,8 +672,10 @@
       <c r="E12">
         <v>4</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F12" s="4"/>
+      <c r="G12" s="4"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>4</v>
       </c>
@@ -651,8 +685,10 @@
       <c r="E13">
         <v>2</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F13" s="4"/>
+      <c r="G13" s="4"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>10</v>
       </c>
@@ -662,8 +698,10 @@
       <c r="E14">
         <v>4</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F14" s="4"/>
+      <c r="G14" s="4"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>11</v>
       </c>
@@ -673,8 +711,10 @@
       <c r="E15">
         <v>3</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F15" s="4"/>
+      <c r="G15" s="4"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>5</v>
       </c>
@@ -684,8 +724,10 @@
       <c r="E16">
         <v>2</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F16" s="4"/>
+      <c r="G16" s="4"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>29</v>
       </c>
@@ -695,8 +737,14 @@
       <c r="E17">
         <v>2</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F17" s="4"/>
+      <c r="G17" s="4"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="F18" s="4"/>
+      <c r="G18" s="4"/>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>8</v>
       </c>
@@ -708,10 +756,13 @@
         <f>SUM(E4:E17)</f>
         <v>40</v>
       </c>
+      <c r="F19" s="4"/>
+      <c r="G19" s="4"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A2:E3"/>
+  <mergeCells count="2">
+    <mergeCell ref="A2:E2"/>
+    <mergeCell ref="A3:E3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>